<commit_message>
regnskap up to date, dokumentert så godt som mulig
</commit_message>
<xml_diff>
--- a/Trekkninger/database.xlsx
+++ b/Trekkninger/database.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="9220" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="9220" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Top 5" sheetId="7" r:id="rId1"/>
@@ -12,8 +12,9 @@
     <sheet name="Lotteries" sheetId="2" r:id="rId3"/>
     <sheet name="Sales" sheetId="3" r:id="rId4"/>
     <sheet name="Prizes" sheetId="4" r:id="rId5"/>
-    <sheet name="new structure" sheetId="10" state="hidden" r:id="rId6"/>
-    <sheet name="Costs" sheetId="9" state="hidden" r:id="rId7"/>
+    <sheet name="Purchases" sheetId="11" r:id="rId6"/>
+    <sheet name="new structure" sheetId="10" state="hidden" r:id="rId7"/>
+    <sheet name="Costs" sheetId="9" state="hidden" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="110">
   <si>
     <t>id</t>
   </si>
@@ -424,7 +425,19 @@
     <t>income</t>
   </si>
   <si>
-    <t>Total</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Purchases</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Saldo?</t>
   </si>
 </sst>
 </file>
@@ -434,7 +447,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -621,7 +634,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -694,6 +707,7 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -718,7 +732,11 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -727,12 +745,52 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="31">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="35" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -742,21 +800,9 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
         <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -837,7 +883,22 @@
       <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -874,43 +935,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <font>
-        <i val="0"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -981,46 +1005,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Persons" displayName="Persons" ref="A1:N46" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Persons" displayName="Persons" ref="A1:N46" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
   <autoFilter ref="A1:N46"/>
   <sortState ref="A2:N46">
     <sortCondition ref="E1:E46"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" name="id" dataDxfId="26"/>
-    <tableColumn id="2" name="name" dataDxfId="25"/>
-    <tableColumn id="3" name="active" dataDxfId="24"/>
-    <tableColumn id="9" name="tickets" dataDxfId="11">
+    <tableColumn id="1" name="id" dataDxfId="28"/>
+    <tableColumn id="2" name="name" dataDxfId="27"/>
+    <tableColumn id="3" name="active" dataDxfId="26"/>
+    <tableColumn id="9" name="tickets" dataDxfId="25">
       <calculatedColumnFormula>SUMIF(Sales!B:B,A2,Sales!D:D)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="#t" dataDxfId="4">
+    <tableColumn id="12" name="#t" dataDxfId="24">
       <calculatedColumnFormula>IF($C2=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D2)+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="prizes" dataDxfId="10">
+    <tableColumn id="10" name="prizes" dataDxfId="23">
       <calculatedColumnFormula>SUMIF(Prizes!B:B,A2,Prizes!D:D)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="#p" dataDxfId="3">
+    <tableColumn id="13" name="#p" dataDxfId="22">
       <calculatedColumnFormula>IF($C2=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F2)+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="sum_μ" dataDxfId="8">
+    <tableColumn id="7" name="sum_μ" dataDxfId="21">
       <calculatedColumnFormula>SUMIF(Sales!B:B,A2,Sales!F:F)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="sum_σ2" dataDxfId="7">
+    <tableColumn id="11" name="sum_σ2" dataDxfId="20">
       <calculatedColumnFormula>SUMIF(Sales!B:B,A2,Sales!G:G)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="luck" dataDxfId="6">
+    <tableColumn id="5" name="luck" dataDxfId="19">
       <calculatedColumnFormula>(F2-H2)/SQRT(I2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="rank" dataDxfId="5">
+    <tableColumn id="6" name="rank" dataDxfId="18">
       <calculatedColumnFormula>IF($C2=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J2)+1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="cost" dataDxfId="23">
+    <tableColumn id="8" name="cost" dataDxfId="17">
       <calculatedColumnFormula>SUMIF(Sales!B:B,A2,Sales!E:E)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="cost/μ" dataDxfId="22">
+    <tableColumn id="4" name="cost/μ" dataDxfId="16">
       <calculatedColumnFormula>L2/H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="#i" dataDxfId="2">
+    <tableColumn id="14" name="#i" dataDxfId="15">
       <calculatedColumnFormula>IF($C2=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M2)+1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1029,25 +1053,25 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Lotteries" displayName="Lotteries" ref="A1:G17" totalsRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Lotteries" displayName="Lotteries" ref="A1:G16">
   <autoFilter ref="A1:G16">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
     <tableColumn id="1" name="id" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="date" dataDxfId="21"/>
-    <tableColumn id="4" name="cost" dataDxfId="20"/>
-    <tableColumn id="3" name="sales" dataDxfId="19">
+    <tableColumn id="2" name="date" dataDxfId="14"/>
+    <tableColumn id="4" name="cost" dataDxfId="13"/>
+    <tableColumn id="3" name="sales" dataDxfId="12">
       <calculatedColumnFormula>SUMIFS(Sales!D:D,Sales!C:C,A2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="prizes" dataDxfId="18">
+    <tableColumn id="5" name="prizes" totalsRowFunction="sum" dataDxfId="11">
       <calculatedColumnFormula>SUMIFS(Prizes!D:D,Prizes!C:C,A2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="income" totalsRowFunction="sum" dataDxfId="1">
+    <tableColumn id="7" name="income" totalsRowFunction="sum" dataDxfId="10">
       <calculatedColumnFormula>Lotteries[[#This Row],[cost]]*Lotteries[[#This Row],[sales]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="µ/ticket" dataDxfId="17" totalsRowDxfId="0">
+    <tableColumn id="6" name="µ/ticket" dataDxfId="9" totalsRowDxfId="0">
       <calculatedColumnFormula>E2/D2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1069,15 +1093,15 @@
   <tableColumns count="7">
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="person_id"/>
-    <tableColumn id="3" name="lottery_id" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="3" name="lottery_id" dataDxfId="8" totalsRowDxfId="7"/>
     <tableColumn id="4" name="tickets"/>
-    <tableColumn id="5" name="cost" dataDxfId="14" totalsRowDxfId="13">
+    <tableColumn id="5" name="cost" dataDxfId="6" totalsRowDxfId="5">
       <calculatedColumnFormula>INDEX(Lotteries!C:C,MATCH(C2,Lotteries!A:A,0))*D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="µ" dataDxfId="12">
+    <tableColumn id="6" name="µ" dataDxfId="4">
       <calculatedColumnFormula>D2*INDEX(Lotteries!G:G,MATCH(C2,Lotteries!A:A,0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="σ2" dataDxfId="9">
+    <tableColumn id="7" name="σ2" dataDxfId="3">
       <calculatedColumnFormula>INDEX(Lotteries!E:E,MATCH(C2,Lotteries!A:A,0))*D2/INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))*(INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))-D2)/INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))*(INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))-INDEX(Lotteries!E:E,MATCH(C2,Lotteries!A:A,0)))/(INDEX(Lotteries!D:D,MATCH(C2,Lotteries!A:A,0))-1)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1102,6 +1126,23 @@
     <tableColumn id="4" name="prizes"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D12" totalsRowShown="0">
+  <autoFilter ref="A1:D12">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" name="id"/>
+    <tableColumn id="2" name="date" dataDxfId="2"/>
+    <tableColumn id="4" name="cost" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="prizes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1371,7 +1412,7 @@
   <dimension ref="B2:S24"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1383,27 +1424,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
       <c r="J2" s="42"/>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52"/>
       <c r="S2" s="43"/>
     </row>
     <row r="3" spans="2:19" ht="16.5" x14ac:dyDescent="0.35">
@@ -1593,27 +1634,27 @@
       <c r="S8" s="16"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="52"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
+      <c r="G10" s="53"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
       <c r="J10" s="44"/>
-      <c r="K10" s="53" t="s">
+      <c r="K10" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="53"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="54"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
       <c r="S10" s="45"/>
     </row>
     <row r="11" spans="2:19" ht="16.5" x14ac:dyDescent="0.35">
@@ -1803,27 +1844,27 @@
       <c r="S16" s="12"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.35">
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="50"/>
       <c r="J18" s="41"/>
-      <c r="K18" s="46" t="s">
+      <c r="K18" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="L18" s="47"/>
-      <c r="M18" s="47"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="47"/>
-      <c r="Q18" s="47"/>
-      <c r="R18" s="47"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="48"/>
       <c r="S18" s="40"/>
     </row>
     <row r="19" spans="2:19" ht="16.5" x14ac:dyDescent="0.35">
@@ -2018,10 +2059,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2039,7 +2080,7 @@
     <col min="17" max="16384" width="8.90625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -2083,7 +2124,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="30">
         <v>8</v>
       </c>
@@ -2098,7 +2139,7 @@
         <v>157</v>
       </c>
       <c r="E2" s="30">
-        <f>IF($C2=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D2)+1)</f>
+        <f t="shared" ref="E2:E46" si="0">IF($C2=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D2)+1)</f>
         <v>1</v>
       </c>
       <c r="F2" s="30">
@@ -2106,7 +2147,7 @@
         <v>8</v>
       </c>
       <c r="G2" s="30">
-        <f>IF($C2=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F2)+1)</f>
+        <f t="shared" ref="G2:G46" si="1">IF($C2=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F2)+1)</f>
         <v>1</v>
       </c>
       <c r="H2" s="31">
@@ -2118,11 +2159,11 @@
         <v>6.1067733955421923</v>
       </c>
       <c r="J2" s="31">
-        <f>(F2-H2)/SQRT(I2)</f>
+        <f t="shared" ref="J2:J46" si="2">(F2-H2)/SQRT(I2)</f>
         <v>0.30226024766922233</v>
       </c>
       <c r="K2" s="30">
-        <f>IF($C2=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J2)+1)</f>
+        <f t="shared" ref="K2:K46" si="3">IF($C2=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J2)+1)</f>
         <v>11</v>
       </c>
       <c r="L2" s="30">
@@ -2130,16 +2171,22 @@
         <v>1740</v>
       </c>
       <c r="M2" s="32">
-        <f>L2/H2</f>
+        <f t="shared" ref="M2:M46" si="4">L2/H2</f>
         <v>239.89881552872043</v>
       </c>
       <c r="N2" s="30">
-        <f>IF($C2=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M2)+1)</f>
-        <v>10</v>
-      </c>
-      <c r="P2" s="54"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+        <f t="shared" ref="N2:N46" si="5">IF($C2=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M2)+1)</f>
+        <v>10</v>
+      </c>
+      <c r="P2" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q2" s="46">
+        <f>INDEX(L:L,MATCH(0,A:A,0))</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="30">
         <v>10</v>
       </c>
@@ -2154,7 +2201,7 @@
         <v>120</v>
       </c>
       <c r="E3" s="30">
-        <f>IF($C3=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D3)+1)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F3" s="30">
@@ -2162,7 +2209,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="30">
-        <f>IF($C3=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F3)+1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H3" s="31">
@@ -2174,11 +2221,11 @@
         <v>4.7415746811763606</v>
       </c>
       <c r="J3" s="31">
-        <f>(F3-H3)/SQRT(I3)</f>
+        <f t="shared" si="2"/>
         <v>-1.0901818568680326</v>
       </c>
       <c r="K3" s="30">
-        <f>IF($C3=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J3)+1)</f>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="L3" s="30">
@@ -2186,15 +2233,15 @@
         <v>1300</v>
       </c>
       <c r="M3" s="32">
-        <f>L3/H3</f>
+        <f t="shared" si="4"/>
         <v>241.91050690099334</v>
       </c>
       <c r="N3" s="30">
-        <f>IF($C3=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M3)+1)</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="30">
         <v>1</v>
       </c>
@@ -2209,7 +2256,7 @@
         <v>102</v>
       </c>
       <c r="E4" s="30">
-        <f>IF($C4=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D4)+1)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F4" s="30">
@@ -2217,7 +2264,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="30">
-        <f>IF($C4=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F4)+1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H4" s="31">
@@ -2229,11 +2276,11 @@
         <v>4.302530692448995</v>
       </c>
       <c r="J4" s="31">
-        <f>(F4-H4)/SQRT(I4)</f>
+        <f t="shared" si="2"/>
         <v>-0.97570370398080453</v>
       </c>
       <c r="K4" s="30">
-        <f>IF($C4=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J4)+1)</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="L4" s="30">
@@ -2241,15 +2288,15 @@
         <v>1110</v>
       </c>
       <c r="M4" s="32">
-        <f>L4/H4</f>
+        <f t="shared" si="4"/>
         <v>220.94575492462749</v>
       </c>
       <c r="N4" s="30">
-        <f>IF($C4=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M4)+1)</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="30">
         <v>37</v>
       </c>
@@ -2264,7 +2311,7 @@
         <v>91</v>
       </c>
       <c r="E5" s="30">
-        <f>IF($C5=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D5)+1)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F5" s="30">
@@ -2272,7 +2319,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="30">
-        <f>IF($C5=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F5)+1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H5" s="31">
@@ -2284,11 +2331,11 @@
         <v>3.6225474141789649</v>
       </c>
       <c r="J5" s="31">
-        <f>(F5-H5)/SQRT(I5)</f>
+        <f t="shared" si="2"/>
         <v>-0.609868477383676</v>
       </c>
       <c r="K5" s="30">
-        <f>IF($C5=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J5)+1)</f>
+        <f t="shared" si="3"/>
         <v>24</v>
       </c>
       <c r="L5" s="30">
@@ -2296,15 +2343,15 @@
         <v>900</v>
       </c>
       <c r="M5" s="32">
-        <f>L5/H5</f>
+        <f t="shared" si="4"/>
         <v>216.30652627574281</v>
       </c>
       <c r="N5" s="30">
-        <f>IF($C5=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M5)+1)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="30">
         <v>33</v>
       </c>
@@ -2319,7 +2366,7 @@
         <v>82</v>
       </c>
       <c r="E6" s="30">
-        <f>IF($C6=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D6)+1)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F6" s="30">
@@ -2327,7 +2374,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="30">
-        <f>IF($C6=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F6)+1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H6" s="31">
@@ -2339,11 +2386,11 @@
         <v>3.3333154045034967</v>
       </c>
       <c r="J6" s="31">
-        <f>(F6-H6)/SQRT(I6)</f>
+        <f t="shared" si="2"/>
         <v>-0.43660492998348149</v>
       </c>
       <c r="K6" s="30">
-        <f>IF($C6=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J6)+1)</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="L6" s="30">
@@ -2351,15 +2398,15 @@
         <v>810</v>
       </c>
       <c r="M6" s="32">
-        <f>L6/H6</f>
+        <f t="shared" si="4"/>
         <v>213.31924534441649</v>
       </c>
       <c r="N6" s="30">
-        <f>IF($C6=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M6)+1)</f>
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="30">
         <v>7</v>
       </c>
@@ -2374,7 +2421,7 @@
         <v>75</v>
       </c>
       <c r="E7" s="30">
-        <f>IF($C7=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D7)+1)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="F7" s="30">
@@ -2382,7 +2429,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="30">
-        <f>IF($C7=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F7)+1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H7" s="31">
@@ -2394,11 +2441,11 @@
         <v>2.7069782274709726</v>
       </c>
       <c r="J7" s="31">
-        <f>(F7-H7)/SQRT(I7)</f>
+        <f t="shared" si="2"/>
         <v>0.55412515952783847</v>
       </c>
       <c r="K7" s="30">
-        <f>IF($C7=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J7)+1)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="L7" s="30">
@@ -2406,15 +2453,15 @@
         <v>800</v>
       </c>
       <c r="M7" s="32">
-        <f>L7/H7</f>
+        <f t="shared" si="4"/>
         <v>259.04189143224175</v>
       </c>
       <c r="N7" s="30">
-        <f>IF($C7=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M7)+1)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="30">
         <v>14</v>
       </c>
@@ -2429,7 +2476,7 @@
         <v>73</v>
       </c>
       <c r="E8" s="30">
-        <f>IF($C8=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D8)+1)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="F8" s="30">
@@ -2437,7 +2484,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="30">
-        <f>IF($C8=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F8)+1)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H8" s="31">
@@ -2449,11 +2496,11 @@
         <v>3.0730745041710636</v>
       </c>
       <c r="J8" s="31">
-        <f>(F8-H8)/SQRT(I8)</f>
+        <f t="shared" si="2"/>
         <v>0.8647466592551053</v>
       </c>
       <c r="K8" s="30">
-        <f>IF($C8=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J8)+1)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="L8" s="30">
@@ -2461,15 +2508,15 @@
         <v>770</v>
       </c>
       <c r="M8" s="32">
-        <f>L8/H8</f>
+        <f t="shared" si="4"/>
         <v>221.0050710785697</v>
       </c>
       <c r="N8" s="30">
-        <f>IF($C8=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M8)+1)</f>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="30">
         <v>24</v>
       </c>
@@ -2484,7 +2531,7 @@
         <v>66</v>
       </c>
       <c r="E9" s="30">
-        <f>IF($C9=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D9)+1)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="F9" s="30">
@@ -2492,7 +2539,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="30">
-        <f>IF($C9=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F9)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H9" s="31">
@@ -2504,11 +2551,11 @@
         <v>2.4399747767702471</v>
       </c>
       <c r="J9" s="31">
-        <f>(F9-H9)/SQRT(I9)</f>
+        <f t="shared" si="2"/>
         <v>-1.1068535147709484</v>
       </c>
       <c r="K9" s="30">
-        <f>IF($C9=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J9)+1)</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="L9" s="30">
@@ -2516,15 +2563,15 @@
         <v>700</v>
       </c>
       <c r="M9" s="32">
-        <f>L9/H9</f>
+        <f t="shared" si="4"/>
         <v>256.50877038767311</v>
       </c>
       <c r="N9" s="30">
-        <f>IF($C9=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M9)+1)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="30">
         <v>5</v>
       </c>
@@ -2539,7 +2586,7 @@
         <v>64</v>
       </c>
       <c r="E10" s="30">
-        <f>IF($C10=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D10)+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F10" s="30">
@@ -2547,7 +2594,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="30">
-        <f>IF($C10=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F10)+1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H10" s="31">
@@ -2559,11 +2606,11 @@
         <v>2.6394415678343002</v>
       </c>
       <c r="J10" s="31">
-        <f>(F10-H10)/SQRT(I10)</f>
+        <f t="shared" si="2"/>
         <v>0.64486200260527571</v>
       </c>
       <c r="K10" s="30">
-        <f>IF($C10=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J10)+1)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="L10" s="30">
@@ -2571,15 +2618,15 @@
         <v>740</v>
       </c>
       <c r="M10" s="32">
-        <f>L10/H10</f>
+        <f t="shared" si="4"/>
         <v>250.64913998317971</v>
       </c>
       <c r="N10" s="30">
-        <f>IF($C10=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M10)+1)</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="30">
         <v>15</v>
       </c>
@@ -2594,7 +2641,7 @@
         <v>64</v>
       </c>
       <c r="E11" s="30">
-        <f>IF($C11=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D11)+1)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="F11" s="30">
@@ -2602,7 +2649,7 @@
         <v>4</v>
       </c>
       <c r="G11" s="30">
-        <f>IF($C11=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F11)+1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H11" s="31">
@@ -2614,11 +2661,11 @@
         <v>3.1295826295726257</v>
       </c>
       <c r="J11" s="31">
-        <f>(F11-H11)/SQRT(I11)</f>
+        <f t="shared" si="2"/>
         <v>0.24142041734861824</v>
       </c>
       <c r="K11" s="30">
-        <f>IF($C11=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J11)+1)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="L11" s="30">
@@ -2626,15 +2673,15 @@
         <v>740</v>
       </c>
       <c r="M11" s="32">
-        <f>L11/H11</f>
+        <f t="shared" si="4"/>
         <v>207.11396393646277</v>
       </c>
       <c r="N11" s="30">
-        <f>IF($C11=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M11)+1)</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="30">
         <v>20</v>
       </c>
@@ -2649,7 +2696,7 @@
         <v>55</v>
       </c>
       <c r="E12" s="30">
-        <f>IF($C12=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D12)+1)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F12" s="30">
@@ -2657,7 +2704,7 @@
         <v>3</v>
       </c>
       <c r="G12" s="30">
-        <f>IF($C12=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F12)+1)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="H12" s="31">
@@ -2669,11 +2716,11 @@
         <v>2.2965397356122015</v>
       </c>
       <c r="J12" s="31">
-        <f>(F12-H12)/SQRT(I12)</f>
+        <f t="shared" si="2"/>
         <v>0.32102335387251679</v>
       </c>
       <c r="K12" s="30">
-        <f>IF($C12=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J12)+1)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="L12" s="30">
@@ -2681,15 +2728,15 @@
         <v>560</v>
       </c>
       <c r="M12" s="32">
-        <f>L12/H12</f>
+        <f t="shared" si="4"/>
         <v>222.79597979541578</v>
       </c>
       <c r="N12" s="30">
-        <f>IF($C12=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M12)+1)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="30">
         <v>29</v>
       </c>
@@ -2704,7 +2751,7 @@
         <v>51</v>
       </c>
       <c r="E13" s="30">
-        <f>IF($C13=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D13)+1)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F13" s="30">
@@ -2712,7 +2759,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="30">
-        <f>IF($C13=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F13)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H13" s="31">
@@ -2724,11 +2771,11 @@
         <v>1.8953049288333335</v>
       </c>
       <c r="J13" s="31">
-        <f>(F13-H13)/SQRT(I13)</f>
+        <f t="shared" si="2"/>
         <v>-0.10114828068400734</v>
       </c>
       <c r="K13" s="30">
-        <f>IF($C13=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J13)+1)</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="L13" s="30">
@@ -2736,15 +2783,15 @@
         <v>500</v>
       </c>
       <c r="M13" s="32">
-        <f>L13/H13</f>
+        <f t="shared" si="4"/>
         <v>233.7266736600364</v>
       </c>
       <c r="N13" s="30">
-        <f>IF($C13=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M13)+1)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="30">
         <v>2</v>
       </c>
@@ -2759,7 +2806,7 @@
         <v>45</v>
       </c>
       <c r="E14" s="30">
-        <f>IF($C14=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D14)+1)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="F14" s="30">
@@ -2767,7 +2814,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="30">
-        <f>IF($C14=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F14)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H14" s="31">
@@ -2779,11 +2826,11 @@
         <v>2.0751785886858025</v>
       </c>
       <c r="J14" s="31">
-        <f>(F14-H14)/SQRT(I14)</f>
+        <f t="shared" si="2"/>
         <v>-0.2247272290975878</v>
       </c>
       <c r="K14" s="30">
-        <f>IF($C14=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J14)+1)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="L14" s="30">
@@ -2791,15 +2838,15 @@
         <v>550</v>
       </c>
       <c r="M14" s="32">
-        <f>L14/H14</f>
+        <f t="shared" si="4"/>
         <v>236.6883905613229</v>
       </c>
       <c r="N14" s="30">
-        <f>IF($C14=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M14)+1)</f>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="30">
         <v>32</v>
       </c>
@@ -2814,7 +2861,7 @@
         <v>41</v>
       </c>
       <c r="E15" s="30">
-        <f>IF($C15=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D15)+1)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F15" s="30">
@@ -2822,7 +2869,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="30">
-        <f>IF($C15=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F15)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H15" s="31">
@@ -2834,11 +2881,11 @@
         <v>1.5500685464079937</v>
       </c>
       <c r="J15" s="31">
-        <f>(F15-H15)/SQRT(I15)</f>
+        <f t="shared" si="2"/>
         <v>0.19973703231952852</v>
       </c>
       <c r="K15" s="30">
-        <f>IF($C15=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J15)+1)</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="L15" s="30">
@@ -2846,15 +2893,15 @@
         <v>400</v>
       </c>
       <c r="M15" s="32">
-        <f>L15/H15</f>
+        <f t="shared" si="4"/>
         <v>228.39864151673595</v>
       </c>
       <c r="N15" s="30">
-        <f>IF($C15=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M15)+1)</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="30">
         <v>36</v>
       </c>
@@ -2869,7 +2916,7 @@
         <v>41</v>
       </c>
       <c r="E16" s="30">
-        <f>IF($C16=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D16)+1)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F16" s="30">
@@ -2877,7 +2924,7 @@
         <v>2</v>
       </c>
       <c r="G16" s="30">
-        <f>IF($C16=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F16)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H16" s="31">
@@ -2889,11 +2936,11 @@
         <v>1.806785994544881</v>
       </c>
       <c r="J16" s="31">
-        <f>(F16-H16)/SQRT(I16)</f>
+        <f t="shared" si="2"/>
         <v>3.1501482295870731E-3</v>
       </c>
       <c r="K16" s="30">
-        <f>IF($C16=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J16)+1)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="L16" s="30">
@@ -2901,11 +2948,11 @@
         <v>400</v>
       </c>
       <c r="M16" s="32">
-        <f>L16/H16</f>
+        <f t="shared" si="4"/>
         <v>200.42433103306936</v>
       </c>
       <c r="N16" s="30">
-        <f>IF($C16=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M16)+1)</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
     </row>
@@ -2924,7 +2971,7 @@
         <v>41</v>
       </c>
       <c r="E17" s="30">
-        <f>IF($C17=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D17)+1)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="F17" s="30">
@@ -2932,7 +2979,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="30">
-        <f>IF($C17=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F17)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H17" s="31">
@@ -2944,11 +2991,11 @@
         <v>1.806785994544881</v>
       </c>
       <c r="J17" s="31">
-        <f>(F17-H17)/SQRT(I17)</f>
+        <f t="shared" si="2"/>
         <v>-0.74080480953425287</v>
       </c>
       <c r="K17" s="30">
-        <f>IF($C17=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J17)+1)</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="L17" s="30">
@@ -2956,11 +3003,11 @@
         <v>400</v>
       </c>
       <c r="M17" s="32">
-        <f>L17/H17</f>
+        <f t="shared" si="4"/>
         <v>200.42433103306936</v>
       </c>
       <c r="N17" s="30">
-        <f>IF($C17=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M17)+1)</f>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
     </row>
@@ -2979,7 +3026,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="30">
-        <f>IF($C18=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D18)+1)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="F18" s="30">
@@ -2987,7 +3034,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="30">
-        <f>IF($C18=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F18)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H18" s="31">
@@ -2999,11 +3046,11 @@
         <v>1.799663023524334</v>
       </c>
       <c r="J18" s="31">
-        <f>(F18-H18)/SQRT(I18)</f>
+        <f t="shared" si="2"/>
         <v>-1.5116432729091189</v>
       </c>
       <c r="K18" s="30">
-        <f>IF($C18=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J18)+1)</f>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="L18" s="30">
@@ -3011,11 +3058,11 @@
         <v>460</v>
       </c>
       <c r="M18" s="32">
-        <f>L18/H18</f>
+        <f t="shared" si="4"/>
         <v>226.83649034053852</v>
       </c>
       <c r="N18" s="30">
-        <f>IF($C18=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M18)+1)</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
@@ -3034,7 +3081,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="30">
-        <f>IF($C19=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D19)+1)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="F19" s="30">
@@ -3042,7 +3089,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="30">
-        <f>IF($C19=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F19)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H19" s="31">
@@ -3054,11 +3101,11 @@
         <v>1.8374415933816806</v>
       </c>
       <c r="J19" s="31">
-        <f>(F19-H19)/SQRT(I19)</f>
+        <f t="shared" si="2"/>
         <v>-0.83309856993406151</v>
       </c>
       <c r="K19" s="30">
-        <f>IF($C19=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J19)+1)</f>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="L19" s="30">
@@ -3066,11 +3113,11 @@
         <v>420</v>
       </c>
       <c r="M19" s="32">
-        <f>L19/H19</f>
+        <f t="shared" si="4"/>
         <v>197.2494075084621</v>
       </c>
       <c r="N19" s="30">
-        <f>IF($C19=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M19)+1)</f>
+        <f t="shared" si="5"/>
         <v>26</v>
       </c>
     </row>
@@ -3089,7 +3136,7 @@
         <v>37</v>
       </c>
       <c r="E20" s="36">
-        <f>IF($C20=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D20)+1)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="F20" s="36">
@@ -3097,7 +3144,7 @@
         <v>4</v>
       </c>
       <c r="G20" s="36">
-        <f>IF($C20=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F20)+1)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H20" s="37">
@@ -3109,11 +3156,11 @@
         <v>1.5474360137130894</v>
       </c>
       <c r="J20" s="37">
-        <f>(F20-H20)/SQRT(I20)</f>
+        <f t="shared" si="2"/>
         <v>1.7963311108174056</v>
       </c>
       <c r="K20" s="38">
-        <f>IF($C20=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J20)+1)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L20" s="36">
@@ -3121,11 +3168,11 @@
         <v>360</v>
       </c>
       <c r="M20" s="32">
-        <f>L20/H20</f>
+        <f t="shared" si="4"/>
         <v>203.9155999000713</v>
       </c>
       <c r="N20" s="30">
-        <f>IF($C20=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M20)+1)</f>
+        <f t="shared" si="5"/>
         <v>22</v>
       </c>
     </row>
@@ -3144,7 +3191,7 @@
         <v>36</v>
       </c>
       <c r="E21" s="30">
-        <f>IF($C21=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D21)+1)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="F21" s="30">
@@ -3152,7 +3199,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="30">
-        <f>IF($C21=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F21)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H21" s="31">
@@ -3164,11 +3211,11 @@
         <v>1.6519362279840033</v>
       </c>
       <c r="J21" s="31">
-        <f>(F21-H21)/SQRT(I21)</f>
+        <f t="shared" si="2"/>
         <v>0.1312620147123815</v>
       </c>
       <c r="K21" s="30">
-        <f>IF($C21=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J21)+1)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="L21" s="30">
@@ -3176,11 +3223,11 @@
         <v>350</v>
       </c>
       <c r="M21" s="32">
-        <f>L21/H21</f>
+        <f t="shared" si="4"/>
         <v>191.12189757643927</v>
       </c>
       <c r="N21" s="30">
-        <f>IF($C21=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M21)+1)</f>
+        <f t="shared" si="5"/>
         <v>28</v>
       </c>
     </row>
@@ -3199,7 +3246,7 @@
         <v>26</v>
       </c>
       <c r="E22" s="30">
-        <f>IF($C22=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D22)+1)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="F22" s="30">
@@ -3207,7 +3254,7 @@
         <v>2</v>
       </c>
       <c r="G22" s="30">
-        <f>IF($C22=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F22)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H22" s="31">
@@ -3219,11 +3266,11 @@
         <v>1.4874787690942293</v>
       </c>
       <c r="J22" s="31">
-        <f>(F22-H22)/SQRT(I22)</f>
+        <f t="shared" si="2"/>
         <v>0.21426238923465521</v>
       </c>
       <c r="K22" s="30">
-        <f>IF($C22=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J22)+1)</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="L22" s="30">
@@ -3231,11 +3278,11 @@
         <v>350</v>
       </c>
       <c r="M22" s="32">
-        <f>L22/H22</f>
+        <f t="shared" si="4"/>
         <v>201.3020454176737</v>
       </c>
       <c r="N22" s="30">
-        <f>IF($C22=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M22)+1)</f>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
     </row>
@@ -3254,7 +3301,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="38">
-        <f>IF($C23=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D23)+1)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="F23" s="36">
@@ -3262,7 +3309,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="38">
-        <f>IF($C23=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F23)+1)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="H23" s="37">
@@ -3274,11 +3321,11 @@
         <v>0.5473464121539795</v>
       </c>
       <c r="J23" s="37">
-        <f>(F23-H23)/SQRT(I23)</f>
+        <f t="shared" si="2"/>
         <v>1.8930256409135764</v>
       </c>
       <c r="K23" s="38">
-        <f>IF($C23=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J23)+1)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L23" s="36">
@@ -3286,11 +3333,11 @@
         <v>150</v>
       </c>
       <c r="M23" s="32">
-        <f>L23/H23</f>
+        <f t="shared" si="4"/>
         <v>250.21459227467813</v>
       </c>
       <c r="N23" s="38">
-        <f>IF($C23=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M23)+1)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
@@ -3309,7 +3356,7 @@
         <v>11</v>
       </c>
       <c r="E24" s="30">
-        <f>IF($C24=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D24)+1)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F24" s="30">
@@ -3317,7 +3364,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="30">
-        <f>IF($C24=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F24)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H24" s="31">
@@ -3329,11 +3376,11 @@
         <v>0.60932526183457325</v>
       </c>
       <c r="J24" s="31">
-        <f>(F24-H24)/SQRT(I24)</f>
+        <f t="shared" si="2"/>
         <v>0.38068025533573507</v>
       </c>
       <c r="K24" s="30">
-        <f>IF($C24=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J24)+1)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="L24" s="30">
@@ -3341,11 +3388,11 @@
         <v>150</v>
       </c>
       <c r="M24" s="32">
-        <f>L24/H24</f>
+        <f t="shared" si="4"/>
         <v>213.41871634405473</v>
       </c>
       <c r="N24" s="30">
-        <f>IF($C24=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M24)+1)</f>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
     </row>
@@ -3364,7 +3411,7 @@
         <v>11</v>
       </c>
       <c r="E25" s="30">
-        <f>IF($C25=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D25)+1)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F25" s="30">
@@ -3372,7 +3419,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="30">
-        <f>IF($C25=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F25)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H25" s="31">
@@ -3384,11 +3431,11 @@
         <v>0.49728853736358486</v>
       </c>
       <c r="J25" s="31">
-        <f>(F25-H25)/SQRT(I25)</f>
+        <f t="shared" si="2"/>
         <v>-0.76198633532411619</v>
       </c>
       <c r="K25" s="30">
-        <f>IF($C25=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J25)+1)</f>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="L25" s="30">
@@ -3396,11 +3443,11 @@
         <v>140</v>
       </c>
       <c r="M25" s="32">
-        <f>L25/H25</f>
+        <f t="shared" si="4"/>
         <v>260.54133138258959</v>
       </c>
       <c r="N25" s="30">
-        <f>IF($C25=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M25)+1)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
@@ -3419,7 +3466,7 @@
         <v>11</v>
       </c>
       <c r="E26" s="30">
-        <f>IF($C26=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D26)+1)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="F26" s="30">
@@ -3427,7 +3474,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="30">
-        <f>IF($C26=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F26)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H26" s="31">
@@ -3439,11 +3486,11 @@
         <v>0.50981180774316925</v>
       </c>
       <c r="J26" s="31">
-        <f>(F26-H26)/SQRT(I26)</f>
+        <f t="shared" si="2"/>
         <v>-0.82094159664369926</v>
       </c>
       <c r="K26" s="30">
-        <f>IF($C26=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J26)+1)</f>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="L26" s="30">
@@ -3451,11 +3498,11 @@
         <v>100</v>
       </c>
       <c r="M26" s="32">
-        <f>L26/H26</f>
+        <f t="shared" si="4"/>
         <v>170.6014795754262</v>
       </c>
       <c r="N26" s="30">
-        <f>IF($C26=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M26)+1)</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
     </row>
@@ -3474,7 +3521,7 @@
         <v>10</v>
       </c>
       <c r="E27" s="36">
-        <f>IF($C27=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D27)+1)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="F27" s="36">
@@ -3482,7 +3529,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="36">
-        <f>IF($C27=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F27)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H27" s="37">
@@ -3494,11 +3541,11 @@
         <v>0.46235499586066903</v>
       </c>
       <c r="J27" s="37">
-        <f>(F27-H27)/SQRT(I27)</f>
+        <f t="shared" si="2"/>
         <v>0.72370413314432125</v>
       </c>
       <c r="K27" s="38">
-        <f>IF($C27=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J27)+1)</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L27" s="36">
@@ -3506,11 +3553,11 @@
         <v>100</v>
       </c>
       <c r="M27" s="32">
-        <f>L27/H27</f>
+        <f t="shared" si="4"/>
         <v>196.88715953307394</v>
       </c>
       <c r="N27" s="30">
-        <f>IF($C27=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M27)+1)</f>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
     </row>
@@ -3529,7 +3576,7 @@
         <v>7</v>
       </c>
       <c r="E28" s="30">
-        <f>IF($C28=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D28)+1)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="F28" s="30">
@@ -3537,7 +3584,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="30">
-        <f>IF($C28=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F28)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H28" s="31">
@@ -3549,11 +3596,11 @@
         <v>0.28688722694915075</v>
       </c>
       <c r="J28" s="31">
-        <f>(F28-H28)/SQRT(I28)</f>
+        <f t="shared" si="2"/>
         <v>-0.57282964535113001</v>
       </c>
       <c r="K28" s="30">
-        <f>IF($C28=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J28)+1)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="L28" s="30">
@@ -3561,11 +3608,11 @@
         <v>90</v>
       </c>
       <c r="M28" s="32">
-        <f>L28/H28</f>
+        <f t="shared" si="4"/>
         <v>293.33333333333331</v>
       </c>
       <c r="N28" s="30">
-        <f>IF($C28=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M28)+1)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3584,7 +3631,7 @@
         <v>6</v>
       </c>
       <c r="E29" s="30">
-        <f>IF($C29=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D29)+1)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="F29" s="30">
@@ -3592,7 +3639,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="30">
-        <f>IF($C29=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F29)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H29" s="31">
@@ -3604,11 +3651,11 @@
         <v>0.45814801658361881</v>
       </c>
       <c r="J29" s="31">
-        <f>(F29-H29)/SQRT(I29)</f>
+        <f t="shared" si="2"/>
         <v>0.67477248464120332</v>
       </c>
       <c r="K29" s="30">
-        <f>IF($C29=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J29)+1)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="L29" s="30">
@@ -3616,11 +3663,11 @@
         <v>100</v>
       </c>
       <c r="M29" s="32">
-        <f>L29/H29</f>
+        <f t="shared" si="4"/>
         <v>184.07079646017698</v>
       </c>
       <c r="N29" s="30">
-        <f>IF($C29=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M29)+1)</f>
+        <f t="shared" si="5"/>
         <v>29</v>
       </c>
     </row>
@@ -3639,7 +3686,7 @@
         <v>5</v>
       </c>
       <c r="E30" s="36">
-        <f>IF($C30=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D30)+1)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="F30" s="36">
@@ -3647,7 +3694,7 @@
         <v>1</v>
       </c>
       <c r="G30" s="36">
-        <f>IF($C30=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F30)+1)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="H30" s="37">
@@ -3659,11 +3706,11 @@
         <v>0.29142171627993935</v>
       </c>
       <c r="J30" s="37">
-        <f>(F30-H30)/SQRT(I30)</f>
+        <f t="shared" si="2"/>
         <v>1.2483688011309693</v>
       </c>
       <c r="K30" s="38">
-        <f>IF($C30=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J30)+1)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="L30" s="36">
@@ -3671,11 +3718,11 @@
         <v>50</v>
       </c>
       <c r="M30" s="32">
-        <f>L30/H30</f>
+        <f t="shared" si="4"/>
         <v>153.33333333333334</v>
       </c>
       <c r="N30" s="30">
-        <f>IF($C30=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M30)+1)</f>
+        <f t="shared" si="5"/>
         <v>31</v>
       </c>
     </row>
@@ -3694,7 +3741,7 @@
         <v>4</v>
       </c>
       <c r="E31" s="36">
-        <f>IF($C31=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D31)+1)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="F31" s="36">
@@ -3702,7 +3749,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="36">
-        <f>IF($C31=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F31)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H31" s="37">
@@ -3714,11 +3761,11 @@
         <v>0.13760129006248742</v>
       </c>
       <c r="J31" s="37">
-        <f>(F31-H31)/SQRT(I31)</f>
+        <f t="shared" si="2"/>
         <v>-0.39211733715048613</v>
       </c>
       <c r="K31" s="38">
-        <f>IF($C31=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J31)+1)</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="L31" s="36">
@@ -3726,11 +3773,11 @@
         <v>40</v>
       </c>
       <c r="M31" s="32">
-        <f>L31/H31</f>
+        <f t="shared" si="4"/>
         <v>275</v>
       </c>
       <c r="N31" s="30">
-        <f>IF($C31=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M31)+1)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
@@ -3749,7 +3796,7 @@
         <v>3</v>
       </c>
       <c r="E32" s="36">
-        <f>IF($C32=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D32)+1)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="F32" s="36">
@@ -3757,7 +3804,7 @@
         <v>0</v>
       </c>
       <c r="G32" s="36">
-        <f>IF($C32=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F32)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H32" s="37">
@@ -3769,11 +3816,11 @@
         <v>0.29810308929110729</v>
       </c>
       <c r="J32" s="37">
-        <f>(F32-H32)/SQRT(I32)</f>
+        <f t="shared" si="2"/>
         <v>-0.66156013751613985</v>
       </c>
       <c r="K32" s="38">
-        <f>IF($C32=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J32)+1)</f>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="L32" s="36">
@@ -3781,11 +3828,11 @@
         <v>20</v>
       </c>
       <c r="M32" s="32">
-        <f>L32/H32</f>
+        <f t="shared" si="4"/>
         <v>55.370370370370374</v>
       </c>
       <c r="N32" s="30">
-        <f>IF($C32=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M32)+1)</f>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
     </row>
@@ -3804,7 +3851,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="30">
-        <f>IF($C33=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D33)+1)</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="F33" s="30">
@@ -3812,7 +3859,7 @@
         <v>0</v>
       </c>
       <c r="G33" s="30">
-        <f>IF($C33=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F33)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H33" s="31">
@@ -3824,11 +3871,11 @@
         <v>6.1462224298748667E-2</v>
       </c>
       <c r="J33" s="31">
-        <f>(F33-H33)/SQRT(I33)</f>
+        <f t="shared" si="2"/>
         <v>-0.25746562908380199</v>
       </c>
       <c r="K33" s="30">
-        <f>IF($C33=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J33)+1)</f>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="L33" s="30">
@@ -3836,11 +3883,11 @@
         <v>20</v>
       </c>
       <c r="M33" s="32">
-        <f>L33/H33</f>
+        <f t="shared" si="4"/>
         <v>313.33333333333337</v>
       </c>
       <c r="N33" s="30">
-        <f>IF($C33=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M33)+1)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -3859,7 +3906,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="36">
-        <f>IF($C34=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D34)+1)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="F34" s="36">
@@ -3867,7 +3914,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="36">
-        <f>IF($C34=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F34)+1)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="H34" s="37">
@@ -3879,11 +3926,11 @@
         <v>0.17751479289940827</v>
       </c>
       <c r="J34" s="37">
-        <f>(F34-H34)/SQRT(I34)</f>
+        <f t="shared" si="2"/>
         <v>-0.54772255750516619</v>
       </c>
       <c r="K34" s="38">
-        <f>IF($C34=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J34)+1)</f>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="L34" s="36">
@@ -3891,11 +3938,11 @@
         <v>0</v>
       </c>
       <c r="M34" s="32">
-        <f>L34/H34</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N34" s="30">
-        <f>IF($C34=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M34)+1)</f>
+        <f t="shared" si="5"/>
         <v>33</v>
       </c>
     </row>
@@ -3914,7 +3961,7 @@
         <v>12</v>
       </c>
       <c r="E35" s="36" t="str">
-        <f>IF($C35=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D35)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F35" s="36">
@@ -3922,7 +3969,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="36" t="str">
-        <f>IF($C35=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F35)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H35" s="37">
@@ -3934,11 +3981,11 @@
         <v>0.81964806980788218</v>
       </c>
       <c r="J35" s="37">
-        <f>(F35-H35)/SQRT(I35)</f>
+        <f t="shared" si="2"/>
         <v>-1.0911366986652986</v>
       </c>
       <c r="K35" s="38" t="str">
-        <f>IF($C35=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J35)+1)</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L35" s="36">
@@ -3946,11 +3993,11 @@
         <v>100</v>
       </c>
       <c r="M35" s="32">
-        <f>L35/H35</f>
+        <f t="shared" si="4"/>
         <v>101.22950819672131</v>
       </c>
       <c r="N35" s="32" t="str">
-        <f>IF($C35=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M35)+1)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3969,7 +4016,7 @@
         <v>55</v>
       </c>
       <c r="E36" s="30" t="str">
-        <f>IF($C36=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D36)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F36" s="30">
@@ -3977,7 +4024,7 @@
         <v>3</v>
       </c>
       <c r="G36" s="30" t="str">
-        <f>IF($C36=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F36)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H36" s="31">
@@ -3989,11 +4036,11 @@
         <v>2.1339918940026701</v>
       </c>
       <c r="J36" s="31">
-        <f>(F36-H36)/SQRT(I36)</f>
+        <f t="shared" si="2"/>
         <v>0.42847177024759042</v>
       </c>
       <c r="K36" s="30" t="str">
-        <f>IF($C36=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J36)+1)</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L36" s="30">
@@ -4001,11 +4048,11 @@
         <v>580</v>
       </c>
       <c r="M36" s="32">
-        <f>L36/H36</f>
+        <f t="shared" si="4"/>
         <v>244.30512797706007</v>
       </c>
       <c r="N36" s="30" t="str">
-        <f>IF($C36=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M36)+1)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4024,7 +4071,7 @@
         <v>25</v>
       </c>
       <c r="E37" s="30" t="str">
-        <f>IF($C37=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D37)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F37" s="30">
@@ -4032,7 +4079,7 @@
         <v>2</v>
       </c>
       <c r="G37" s="30" t="str">
-        <f>IF($C37=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F37)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H37" s="31">
@@ -4044,11 +4091,11 @@
         <v>1.4304524128940306</v>
       </c>
       <c r="J37" s="31">
-        <f>(F37-H37)/SQRT(I37)</f>
+        <f t="shared" si="2"/>
         <v>0.29081541460884686</v>
       </c>
       <c r="K37" s="30" t="str">
-        <f>IF($C37=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J37)+1)</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L37" s="30">
@@ -4056,11 +4103,11 @@
         <v>350</v>
       </c>
       <c r="M37" s="32">
-        <f>L37/H37</f>
+        <f t="shared" si="4"/>
         <v>211.8412815677431</v>
       </c>
       <c r="N37" s="32" t="str">
-        <f>IF($C37=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M37)+1)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4079,7 +4126,7 @@
         <v>68</v>
       </c>
       <c r="E38" s="30" t="str">
-        <f>IF($C38=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D38)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F38" s="30">
@@ -4087,7 +4134,7 @@
         <v>7</v>
       </c>
       <c r="G38" s="30" t="str">
-        <f>IF($C38=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F38)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H38" s="31">
@@ -4099,11 +4146,11 @@
         <v>2.8574411080798878</v>
       </c>
       <c r="J38" s="31">
-        <f>(F38-H38)/SQRT(I38)</f>
+        <f t="shared" si="2"/>
         <v>2.224200373221318</v>
       </c>
       <c r="K38" s="30" t="str">
-        <f>IF($C38=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J38)+1)</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L38" s="30">
@@ -4111,11 +4158,11 @@
         <v>720</v>
       </c>
       <c r="M38" s="32">
-        <f>L38/H38</f>
+        <f t="shared" si="4"/>
         <v>222.20720539888777</v>
       </c>
       <c r="N38" s="30" t="str">
-        <f>IF($C38=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M38)+1)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4134,7 +4181,7 @@
         <v>48</v>
       </c>
       <c r="E39" s="30" t="str">
-        <f>IF($C39=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D39)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F39" s="30">
@@ -4142,7 +4189,7 @@
         <v>3</v>
       </c>
       <c r="G39" s="30" t="str">
-        <f>IF($C39=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F39)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H39" s="31">
@@ -4154,11 +4201,11 @@
         <v>1.9505675531744411</v>
       </c>
       <c r="J39" s="31">
-        <f>(F39-H39)/SQRT(I39)</f>
+        <f t="shared" si="2"/>
         <v>0.59821503232865181</v>
       </c>
       <c r="K39" s="30" t="str">
-        <f>IF($C39=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J39)+1)</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L39" s="30">
@@ -4166,11 +4213,11 @@
         <v>530</v>
       </c>
       <c r="M39" s="32">
-        <f>L39/H39</f>
+        <f t="shared" si="4"/>
         <v>244.85836578291148</v>
       </c>
       <c r="N39" s="30" t="str">
-        <f>IF($C39=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M39)+1)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4189,7 +4236,7 @@
         <v>147</v>
       </c>
       <c r="E40" s="30" t="str">
-        <f>IF($C40=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D40)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F40" s="30">
@@ -4197,7 +4244,7 @@
         <v>4</v>
       </c>
       <c r="G40" s="30" t="str">
-        <f>IF($C40=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F40)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H40" s="31">
@@ -4209,11 +4256,11 @@
         <v>4.614036279068543</v>
       </c>
       <c r="J40" s="31">
-        <f>(F40-H40)/SQRT(I40)</f>
+        <f t="shared" si="2"/>
         <v>-0.6458180421064228</v>
       </c>
       <c r="K40" s="30" t="str">
-        <f>IF($C40=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J40)+1)</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L40" s="30">
@@ -4221,11 +4268,11 @@
         <v>1570</v>
       </c>
       <c r="M40" s="32">
-        <f>L40/H40</f>
+        <f t="shared" si="4"/>
         <v>291.4295377006145</v>
       </c>
       <c r="N40" s="32" t="str">
-        <f>IF($C40=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M40)+1)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4244,7 +4291,7 @@
         <v>15</v>
       </c>
       <c r="E41" s="30" t="str">
-        <f>IF($C41=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D41)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F41" s="30">
@@ -4252,7 +4299,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="30" t="str">
-        <f>IF($C41=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F41)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H41" s="31">
@@ -4264,11 +4311,11 @@
         <v>0.57472666253306171</v>
       </c>
       <c r="J41" s="31">
-        <f>(F41-H41)/SQRT(I41)</f>
+        <f t="shared" si="2"/>
         <v>0.4858824982778579</v>
       </c>
       <c r="K41" s="30" t="str">
-        <f>IF($C41=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J41)+1)</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L41" s="30">
@@ -4276,11 +4323,11 @@
         <v>200</v>
       </c>
       <c r="M41" s="32">
-        <f>L41/H41</f>
+        <f t="shared" si="4"/>
         <v>316.6315789473685</v>
       </c>
       <c r="N41" s="30" t="str">
-        <f>IF($C41=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M41)+1)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4299,7 +4346,7 @@
         <v>75</v>
       </c>
       <c r="E42" s="30" t="str">
-        <f>IF($C42=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D42)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F42" s="30">
@@ -4307,7 +4354,7 @@
         <v>4</v>
       </c>
       <c r="G42" s="30" t="str">
-        <f>IF($C42=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F42)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H42" s="31">
@@ -4319,11 +4366,11 @@
         <v>2.6922037778817822</v>
       </c>
       <c r="J42" s="31">
-        <f>(F42-H42)/SQRT(I42)</f>
+        <f t="shared" si="2"/>
         <v>0.61000837120979057</v>
       </c>
       <c r="K42" s="30" t="str">
-        <f>IF($C42=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J42)+1)</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L42" s="30">
@@ -4331,11 +4378,11 @@
         <v>800</v>
       </c>
       <c r="M42" s="32">
-        <f>L42/H42</f>
+        <f t="shared" si="4"/>
         <v>266.74650011229147</v>
       </c>
       <c r="N42" s="30" t="str">
-        <f>IF($C42=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M42)+1)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4354,7 +4401,7 @@
         <v>10</v>
       </c>
       <c r="E43" s="30" t="str">
-        <f>IF($C43=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D43)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F43" s="30">
@@ -4362,7 +4409,7 @@
         <v>0</v>
       </c>
       <c r="G43" s="30" t="str">
-        <f>IF($C43=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F43)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H43" s="31">
@@ -4374,11 +4421,11 @@
         <v>0.2940934388488512</v>
       </c>
       <c r="J43" s="31">
-        <f>(F43-H43)/SQRT(I43)</f>
+        <f t="shared" si="2"/>
         <v>-0.58850578094375816</v>
       </c>
       <c r="K43" s="30" t="str">
-        <f>IF($C43=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J43)+1)</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L43" s="30">
@@ -4386,11 +4433,11 @@
         <v>100</v>
       </c>
       <c r="M43" s="32">
-        <f>L43/H43</f>
+        <f t="shared" si="4"/>
         <v>313.33333333333337</v>
       </c>
       <c r="N43" s="32" t="str">
-        <f>IF($C43=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M43)+1)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4409,7 +4456,7 @@
         <v>24</v>
       </c>
       <c r="E44" s="30" t="str">
-        <f>IF($C44=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D44)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F44" s="30">
@@ -4417,7 +4464,7 @@
         <v>0</v>
       </c>
       <c r="G44" s="30" t="str">
-        <f>IF($C44=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F44)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H44" s="31">
@@ -4429,11 +4476,11 @@
         <v>0.74063394841795605</v>
       </c>
       <c r="J44" s="31">
-        <f>(F44-H44)/SQRT(I44)</f>
+        <f t="shared" si="2"/>
         <v>-0.92277706012539296</v>
       </c>
       <c r="K44" s="30" t="str">
-        <f>IF($C44=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J44)+1)</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L44" s="30">
@@ -4441,11 +4488,11 @@
         <v>240</v>
       </c>
       <c r="M44" s="32">
-        <f>L44/H44</f>
+        <f t="shared" si="4"/>
         <v>302.21265389966049</v>
       </c>
       <c r="N44" s="32" t="str">
-        <f>IF($C44=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M44)+1)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4464,7 +4511,7 @@
         <v>5</v>
       </c>
       <c r="E45" s="30" t="str">
-        <f>IF($C45=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D45)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F45" s="30">
@@ -4472,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="30" t="str">
-        <f>IF($C45=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F45)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H45" s="31">
@@ -4484,11 +4531,11 @@
         <v>0.19294176003734828</v>
       </c>
       <c r="J45" s="31">
-        <f>(F45-H45)/SQRT(I45)</f>
+        <f t="shared" si="2"/>
         <v>-0.47429183107111794</v>
       </c>
       <c r="K45" s="30" t="str">
-        <f>IF($C45=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J45)+1)</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L45" s="30">
@@ -4496,11 +4543,11 @@
         <v>50</v>
       </c>
       <c r="M45" s="32">
-        <f>L45/H45</f>
+        <f t="shared" si="4"/>
         <v>240.00000000000003</v>
       </c>
       <c r="N45" s="32" t="str">
-        <f>IF($C45=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M45)+1)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4519,7 +4566,7 @@
         <v>16</v>
       </c>
       <c r="E46" s="30" t="str">
-        <f>IF($C46=0," ",COUNTIFS($C:$C,1,D:D,"&gt;"&amp;D46)+1)</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="F46" s="30">
@@ -4527,7 +4574,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="30" t="str">
-        <f>IF($C46=0," ",COUNTIFS($C:$C,1,F:F,"&gt;"&amp;F46)+1)</f>
+        <f t="shared" si="1"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H46" s="31">
@@ -4539,11 +4586,11 @@
         <v>0.63196321395379162</v>
       </c>
       <c r="J46" s="31">
-        <f>(F46-H46)/SQRT(I46)</f>
+        <f t="shared" si="2"/>
         <v>0.39856301064268529</v>
       </c>
       <c r="K46" s="30" t="str">
-        <f>IF($C46=0," ",COUNTIFS($C:$C,1,J:J,"&gt;"&amp;J46)+1)</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="L46" s="30">
@@ -4551,11 +4598,11 @@
         <v>160</v>
       </c>
       <c r="M46" s="32">
-        <f>L46/H46</f>
+        <f t="shared" si="4"/>
         <v>234.20647149460706</v>
       </c>
       <c r="N46" s="32" t="str">
-        <f>IF($C46=0," ",COUNTIFS($C:$C,1,M:M,"&gt;"&amp;M46)+1)</f>
+        <f t="shared" si="5"/>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4569,10 +4616,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5009,16 +5056,6 @@
         <v>6.5217391304347824E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F17">
-        <f>SUBTOTAL(109,Lotteries[income])</f>
-        <v>20720</v>
-      </c>
-      <c r="G17" s="4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -5029,10 +5066,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J274"/>
+  <dimension ref="A1:K274"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B261" sqref="B261"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5040,9 +5077,10 @@
     <col min="2" max="2" width="11.1796875" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="8" max="8" width="8.90625" style="2"/>
+    <col min="10" max="11" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5065,7 +5103,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5093,8 +5131,15 @@
       <c r="H2" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K2" s="55">
+        <f>SUM(E:E)</f>
+        <v>20720</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5123,7 +5168,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5152,7 +5197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5181,7 +5226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5210,7 +5255,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5239,7 +5284,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5268,7 +5313,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5297,7 +5342,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5326,7 +5371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5355,7 +5400,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5384,7 +5429,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5413,7 +5458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5442,7 +5487,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5471,7 +5516,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -14515,6 +14560,232 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.90625" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.08984375" style="55" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>42291</v>
+      </c>
+      <c r="C2" s="56">
+        <v>1651.2</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="55">
+        <v>3929</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>42412</v>
+      </c>
+      <c r="C3" s="56">
+        <v>986.65</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="55">
+        <f>Sales!K2</f>
+        <v>20720</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>42482</v>
+      </c>
+      <c r="C4" s="56">
+        <v>1083.5</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="55">
+        <f>-Persons!Q2</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43173</v>
+      </c>
+      <c r="C5" s="56">
+        <v>2500</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="F5" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="58">
+        <f>-SUM(C:C)</f>
+        <v>-20124.150000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>43255</v>
+      </c>
+      <c r="C6" s="56">
+        <v>2599</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="G6" s="55">
+        <f>SUM(G2:G5)</f>
+        <v>4424.8499999999985</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="56">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>43333</v>
+      </c>
+      <c r="C8" s="56">
+        <v>2744</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>43420</v>
+      </c>
+      <c r="C9" s="56">
+        <v>2493</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>43447</v>
+      </c>
+      <c r="C10" s="56">
+        <v>535.79999999999995</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>43476</v>
+      </c>
+      <c r="C11" s="56">
+        <v>2637</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>43538</v>
+      </c>
+      <c r="C12" s="56">
+        <v>2894</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14648,7 +14919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1"/>
   <sheetViews>

</xml_diff>